<commit_message>
Agregado modo On Off by time
Permite encender y apagar (0-100%) segun la hora sin
definir toda una curva.
</commit_message>
<xml_diff>
--- a/Docs/Comandos.xlsx
+++ b/Docs/Comandos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Agustin\Documents\AGUSTIN\Promatix\medidores la rural\firmware\SmartCell-xDot-v2_uvision6_xdot_l151cc\SmartCell-xDot-v2\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588CB54E-A8A7-4574-8648-FAC44C633F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8611E8B-00F0-4604-9259-626DBED13C4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1394AEC9-9D6B-417F-AB39-DF4639FF308A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
   <si>
     <t>Comandos Uplink</t>
   </si>
@@ -339,6 +339,24 @@
   </si>
   <si>
     <t>Byte mas significativo primero</t>
+  </si>
+  <si>
+    <t>On Off por tiempo</t>
+  </si>
+  <si>
+    <t>Set hora on-off</t>
+  </si>
+  <si>
+    <t>Hora on</t>
+  </si>
+  <si>
+    <t>Minuto on</t>
+  </si>
+  <si>
+    <t>Hora off</t>
+  </si>
+  <si>
+    <t>Minuto off</t>
   </si>
 </sst>
 </file>
@@ -453,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -467,14 +485,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -482,10 +506,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,7 +823,7 @@
   <dimension ref="A2:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,41 +835,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="8" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
@@ -868,7 +888,7 @@
       <c r="H5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -895,7 +915,7 @@
       <c r="H6" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -922,7 +942,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -949,7 +969,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -969,10 +989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A081C0C-1C07-4C39-96BD-43EE206A4844}">
-  <dimension ref="A2:K24"/>
+  <dimension ref="A2:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,73 +1001,77 @@
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="59.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1058,19 +1082,23 @@
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="1" t="str">
+        <f>DEC2HEX(CODE(D6),2)</f>
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -1081,282 +1109,364 @@
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="1" t="str">
+        <f t="shared" ref="E7:E17" si="0">DEC2HEX(CODE(D7),2)</f>
+        <v>44</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4F</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4D</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>89</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>79</v>
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4A</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4B</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="6" t="s">
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C21" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D24" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D25" s="1">
         <v>3</v>
+      </c>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C2:I2"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="F4:K4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Separacion entre loops de transmision y loops de medicion
El loop principal se ejecuta con poco tiempo de diferencia
(30s), pero solo se habilita la transmision cada cierto
numero (20) de ciclos.
</commit_message>
<xml_diff>
--- a/Docs/Comandos.xlsx
+++ b/Docs/Comandos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Agustin\Documents\AGUSTIN\Promatix\medidores la rural\firmware\SmartCell-xDot-v2_uvision6_xdot_l151cc\SmartCell-xDot-v2\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8611E8B-00F0-4604-9259-626DBED13C4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCDB93D-5263-4FD8-AB18-B891E189132B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1394AEC9-9D6B-417F-AB39-DF4639FF308A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
   <si>
     <t>Comandos Uplink</t>
   </si>
@@ -357,6 +357,15 @@
   </si>
   <si>
     <t>Minuto off</t>
+  </si>
+  <si>
+    <t>loop delay(0)</t>
+  </si>
+  <si>
+    <t>loop delay(1)</t>
+  </si>
+  <si>
+    <t>loops to send</t>
   </si>
 </sst>
 </file>
@@ -991,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A081C0C-1C07-4C39-96BD-43EE206A4844}">
   <dimension ref="A2:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,9 +1383,15 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>

</xml_diff>

<commit_message>
El guardado en memoria no volatil se hace fuera del payloadParser
Los uplinks son no confirmados.
</commit_message>
<xml_diff>
--- a/Docs/Comandos.xlsx
+++ b/Docs/Comandos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Agustin\Documents\AGUSTIN\Promatix\medidores la rural\firmware\SmartCell-xDot-v2_uvision6_xdot_l151cc\SmartCell-xDot-v2\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCDB93D-5263-4FD8-AB18-B891E189132B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9CB001-4660-4943-A941-C1CD272D5385}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1394AEC9-9D6B-417F-AB39-DF4639FF308A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
   <si>
     <t>Comandos Uplink</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>loops to send</t>
+  </si>
+  <si>
+    <t>hex</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1004,7 @@
   <dimension ref="A2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1060,9 @@
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="F5" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>